<commit_message>
Break point location tables
</commit_message>
<xml_diff>
--- a/tables/table7_ssy-break-points.xlsx
+++ b/tables/table7_ssy-break-points.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -370,11 +370,6 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>PettittP</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
           <t>TaylorBreak</t>
         </is>
       </c>
@@ -385,13 +380,12 @@
           <t>Apchas</t>
         </is>
       </c>
-      <c r="B2">
-        <v>2000</v>
-      </c>
-      <c r="C2">
-        <v>0.0003553751977543359</v>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2000*</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>2001 (1987–2003)</t>
         </is>
@@ -403,13 +397,12 @@
           <t>Belaya (No. 83361)</t>
         </is>
       </c>
-      <c r="B3">
-        <v>1999</v>
-      </c>
-      <c r="C3">
-        <v>0.007732022892083986</v>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1999*</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>1967 (1932–1975)</t>
         </is>
@@ -421,13 +414,12 @@
           <t>Kuban (No. 83174)</t>
         </is>
       </c>
-      <c r="B4">
-        <v>1999</v>
-      </c>
-      <c r="C4">
-        <v>5.91160728541371E-05</v>
-      </c>
-      <c r="D4" t="inlineStr">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1999*</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>1969 (1943–1971)</t>
         </is>
@@ -439,13 +431,12 @@
           <t>Laba (No. 83314)</t>
         </is>
       </c>
-      <c r="B5">
-        <v>1966</v>
-      </c>
-      <c r="C5">
-        <v>0.0007835040757608419</v>
-      </c>
-      <c r="D5" t="inlineStr">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1966*</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>1967 (1940–1968)</t>
         </is>
@@ -457,13 +448,12 @@
           <t>Laba (No. 83314)</t>
         </is>
       </c>
-      <c r="B6">
-        <v>1966</v>
-      </c>
-      <c r="C6">
-        <v>0.0007835040757608419</v>
-      </c>
-      <c r="D6" t="inlineStr">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1966*</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
         <is>
           <t>1981 (1977–1995)</t>
         </is>
@@ -475,13 +465,12 @@
           <t>Marta</t>
         </is>
       </c>
-      <c r="B7">
-        <v>1999</v>
-      </c>
-      <c r="C7">
-        <v>0.0005379970523469576</v>
-      </c>
-      <c r="D7" t="inlineStr">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1999*</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t>2001 (1984–2003)</t>
         </is>
@@ -493,13 +482,12 @@
           <t>Psekups</t>
         </is>
       </c>
-      <c r="B8">
-        <v>2001</v>
-      </c>
-      <c r="C8">
-        <v>0.0005379970523469576</v>
-      </c>
-      <c r="D8" t="inlineStr">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2001*</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>2003 (1990–2005)</t>
         </is>
@@ -511,13 +499,12 @@
           <t>Pshish (No. 83387)</t>
         </is>
       </c>
-      <c r="B9">
-        <v>1999</v>
-      </c>
-      <c r="C9">
-        <v>6.109489651521639E-05</v>
-      </c>
-      <c r="D9" t="inlineStr">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1999*</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
         <is>
           <t>1960 (1957–1962)</t>
         </is>
@@ -529,13 +516,12 @@
           <t>Pshish (No. 83387)</t>
         </is>
       </c>
-      <c r="B10">
-        <v>1999</v>
-      </c>
-      <c r="C10">
-        <v>6.109489651521639E-05</v>
-      </c>
-      <c r="D10" t="inlineStr">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1999*</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
         <is>
           <t>1981 (1978–1981)</t>
         </is>
@@ -547,13 +533,12 @@
           <t>Pshish (No. 83387)</t>
         </is>
       </c>
-      <c r="B11">
-        <v>1999</v>
-      </c>
-      <c r="C11">
-        <v>6.109489651521639E-05</v>
-      </c>
-      <c r="D11" t="inlineStr">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1999*</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
         <is>
           <t>2001 (2001–2003)</t>
         </is>
@@ -565,13 +550,12 @@
           <t>Shunduk</t>
         </is>
       </c>
-      <c r="B12">
-        <v>2000</v>
-      </c>
-      <c r="C12">
-        <v>0.0006406282060156441</v>
-      </c>
-      <c r="D12" t="inlineStr">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2000*</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
         <is>
           <t>2001 (1979–2004)</t>
         </is>

</xml_diff>